<commit_message>
Update AllHome Gapan Transmittal(Printer Replacement)_02_01_2021.xlsx
</commit_message>
<xml_diff>
--- a/AllHome Gapan Transmittal(Printer Replacement)_02_01_2021.xlsx
+++ b/AllHome Gapan Transmittal(Printer Replacement)_02_01_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UBIVELOX\Documents\GitHub\Transmittal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10896797-3CF0-4C29-9672-71971E815993}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FAB08F4-139A-428F-801F-07949D49BDF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="6300" yWindow="4524" windowWidth="17088" windowHeight="8328" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -155,12 +155,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -704,7 +711,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -714,17 +721,17 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
@@ -745,180 +752,180 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="12" fontId="13" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="12" fontId="12" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
@@ -930,13 +937,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
@@ -945,8 +952,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -954,7 +964,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -963,25 +973,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1676,16 +1683,16 @@
     <row r="3" spans="1:20" ht="28.2">
       <c r="A3" s="24"/>
       <c r="B3" s="25"/>
-      <c r="C3" s="84" t="s">
+      <c r="C3" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="85"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="75"/>
     </row>
     <row r="4" spans="1:20" ht="28.2">
       <c r="A4" s="26"/>
@@ -1712,77 +1719,77 @@
       <c r="J5" s="14"/>
     </row>
     <row r="6" spans="1:20" ht="15" customHeight="1">
-      <c r="A6" s="73" t="s">
+      <c r="A6" s="82" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="86" t="s">
+      <c r="D6" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="86"/>
-      <c r="J6" s="87"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="77"/>
     </row>
     <row r="7" spans="1:20" ht="15" customHeight="1">
-      <c r="A7" s="73"/>
+      <c r="A7" s="82"/>
       <c r="B7" s="13"/>
       <c r="C7" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="86" t="s">
+      <c r="D7" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="86"/>
-      <c r="F7" s="86"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="86"/>
-      <c r="I7" s="86"/>
-      <c r="J7" s="87"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="77"/>
     </row>
     <row r="8" spans="1:20">
-      <c r="A8" s="73"/>
+      <c r="A8" s="82"/>
       <c r="B8" s="13"/>
       <c r="C8" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="74">
+      <c r="D8" s="78">
         <v>42836</v>
       </c>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
-      <c r="H8" s="75"/>
-      <c r="I8" s="75"/>
-      <c r="J8" s="76"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="79"/>
+      <c r="I8" s="79"/>
+      <c r="J8" s="80"/>
       <c r="M8" s="13"/>
-      <c r="N8" s="72"/>
-      <c r="O8" s="72"/>
-      <c r="P8" s="72"/>
-      <c r="Q8" s="72"/>
+      <c r="N8" s="81"/>
+      <c r="O8" s="81"/>
+      <c r="P8" s="81"/>
+      <c r="Q8" s="81"/>
       <c r="R8" s="13"/>
       <c r="S8" s="13"/>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="73"/>
+      <c r="A9" s="82"/>
       <c r="B9" s="13"/>
       <c r="C9" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="74" t="s">
+      <c r="D9" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="76"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="79"/>
+      <c r="J9" s="80"/>
       <c r="M9" s="13"/>
       <c r="N9" s="13"/>
       <c r="O9" s="13"/>
@@ -1792,7 +1799,7 @@
       <c r="S9" s="13"/>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="73"/>
+      <c r="A10" s="82"/>
       <c r="B10" s="13"/>
       <c r="C10" s="29"/>
       <c r="D10" s="30"/>
@@ -1816,13 +1823,13 @@
       </c>
       <c r="B11" s="13"/>
       <c r="C11" s="34"/>
-      <c r="D11" s="77"/>
-      <c r="E11" s="77"/>
-      <c r="F11" s="77"/>
-      <c r="G11" s="77"/>
-      <c r="H11" s="77"/>
-      <c r="I11" s="77"/>
-      <c r="J11" s="78"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="83"/>
+      <c r="F11" s="83"/>
+      <c r="G11" s="83"/>
+      <c r="H11" s="83"/>
+      <c r="I11" s="83"/>
+      <c r="J11" s="84"/>
       <c r="M11" s="13"/>
       <c r="N11" s="13"/>
       <c r="O11" s="59"/>
@@ -1837,15 +1844,15 @@
       <c r="C12" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="79" t="s">
+      <c r="D12" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="80"/>
-      <c r="F12" s="80"/>
-      <c r="G12" s="80"/>
-      <c r="H12" s="80"/>
-      <c r="I12" s="80"/>
-      <c r="J12" s="81"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="86"/>
+      <c r="I12" s="86"/>
+      <c r="J12" s="87"/>
       <c r="O12" s="60"/>
     </row>
     <row r="13" spans="1:20" ht="19.5" customHeight="1">
@@ -1873,9 +1880,9 @@
       <c r="I14" s="42"/>
       <c r="J14" s="62"/>
       <c r="O14" s="60"/>
-      <c r="R14" s="82"/>
-      <c r="S14" s="82"/>
-      <c r="T14" s="82"/>
+      <c r="R14" s="72"/>
+      <c r="S14" s="72"/>
+      <c r="T14" s="72"/>
     </row>
     <row r="15" spans="1:20" ht="22.5" customHeight="1">
       <c r="A15" s="33"/>
@@ -2365,14 +2372,14 @@
     <row r="48" spans="1:15" ht="28.2">
       <c r="A48" s="55"/>
       <c r="B48" s="13"/>
-      <c r="C48" s="83"/>
-      <c r="D48" s="83"/>
-      <c r="E48" s="83"/>
-      <c r="F48" s="83"/>
-      <c r="G48" s="83"/>
-      <c r="H48" s="83"/>
-      <c r="I48" s="83"/>
-      <c r="J48" s="83"/>
+      <c r="C48" s="73"/>
+      <c r="D48" s="73"/>
+      <c r="E48" s="73"/>
+      <c r="F48" s="73"/>
+      <c r="G48" s="73"/>
+      <c r="H48" s="73"/>
+      <c r="I48" s="73"/>
+      <c r="J48" s="73"/>
     </row>
     <row r="49" spans="1:17">
       <c r="A49" s="56"/>
@@ -2421,10 +2428,10 @@
       <c r="H52" s="56"/>
       <c r="I52" s="56"/>
       <c r="J52" s="56"/>
-      <c r="N52" s="72"/>
-      <c r="O52" s="72"/>
-      <c r="P52" s="72"/>
-      <c r="Q52" s="72"/>
+      <c r="N52" s="81"/>
+      <c r="O52" s="81"/>
+      <c r="P52" s="81"/>
+      <c r="Q52" s="81"/>
     </row>
     <row r="53" spans="1:17">
       <c r="A53" s="56"/>
@@ -2682,6 +2689,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="N52:Q52"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="D9:J9"/>
+    <mergeCell ref="D11:J11"/>
+    <mergeCell ref="D12:J12"/>
     <mergeCell ref="R14:T14"/>
     <mergeCell ref="C48:J48"/>
     <mergeCell ref="C3:J3"/>
@@ -2689,13 +2701,8 @@
     <mergeCell ref="D7:J7"/>
     <mergeCell ref="D8:J8"/>
     <mergeCell ref="N8:Q8"/>
-    <mergeCell ref="N52:Q52"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="D9:J9"/>
-    <mergeCell ref="D11:J11"/>
-    <mergeCell ref="D12:J12"/>
   </mergeCells>
-  <phoneticPr fontId="21" type="noConversion"/>
+  <phoneticPr fontId="22" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="64" orientation="portrait" verticalDpi="300" r:id="rId1"/>
@@ -2711,7 +2718,7 @@
   <dimension ref="A2:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A8" zoomScale="130" zoomScaleNormal="85" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B15" sqref="B15:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -2766,12 +2773,12 @@
       <c r="A10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="111" t="s">
+      <c r="B10" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="100"/>
-      <c r="D10" s="100"/>
-      <c r="E10" s="101"/>
+      <c r="C10" s="101"/>
+      <c r="D10" s="101"/>
+      <c r="E10" s="102"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
@@ -2781,12 +2788,12 @@
       <c r="A11" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="102" t="s">
+      <c r="B11" s="103" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="103"/>
-      <c r="D11" s="103"/>
-      <c r="E11" s="104"/>
+      <c r="C11" s="104"/>
+      <c r="D11" s="104"/>
+      <c r="E11" s="105"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
@@ -2796,12 +2803,12 @@
       <c r="A12" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="105">
+      <c r="B12" s="106">
         <v>44198</v>
       </c>
-      <c r="C12" s="106"/>
-      <c r="D12" s="106"/>
-      <c r="E12" s="107"/>
+      <c r="C12" s="107"/>
+      <c r="D12" s="107"/>
+      <c r="E12" s="108"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
@@ -2811,12 +2818,12 @@
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="108" t="s">
+      <c r="B13" s="109" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="109"/>
-      <c r="D13" s="109"/>
-      <c r="E13" s="110"/>
+      <c r="C13" s="110"/>
+      <c r="D13" s="110"/>
+      <c r="E13" s="111"/>
     </row>
     <row r="14" spans="1:10" ht="15.6">
       <c r="A14" s="10" t="s">
@@ -2997,7 +3004,7 @@
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B13:E13"/>
   </mergeCells>
-  <phoneticPr fontId="21" type="noConversion"/>
+  <phoneticPr fontId="22" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.45" top="1" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>